<commit_message>
range and start correction
</commit_message>
<xml_diff>
--- a/Domestic Standard Upload Tmplt.xlsx
+++ b/Domestic Standard Upload Tmplt.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\275261\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC53CE06-312B-4614-8151-FA1A9D504034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{CC53CE06-312B-4614-8151-FA1A9D504034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB205CAE-2EC9-49D5-8AD4-9B3D155343CD}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="1" activeTab="1" xr2:uid="{CE78BDE3-7438-4330-9B0A-3EEE37903C7F}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" firstSheet="2" activeTab="2" xr2:uid="{CE78BDE3-7438-4330-9B0A-3EEE37903C7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Combined Master" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Dmstc Stndrd Upld Tmplt" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Combined Master'!$A$1:$K$101</definedName>
+    <definedName name="budgetmonth">Sheet1!$A$2:$A$2</definedName>
     <definedName name="category">'Dmstc Stndrd Upld Tmplt'!$L$5</definedName>
     <definedName name="class">'Dmstc Stndrd Upld Tmplt'!$K$5</definedName>
     <definedName name="classx">'Dmstc Stndrd Upld Tmplt'!$K$5</definedName>
@@ -35,6 +37,7 @@
     <definedName name="size">'Dmstc Stndrd Upld Tmplt'!$F$5</definedName>
     <definedName name="supplierid">'Dmstc Stndrd Upld Tmplt'!$I$5</definedName>
     <definedName name="test">'Dmstc Stndrd Upld Tmplt'!$K$5</definedName>
+    <definedName name="testrange">Sheet1!$C$6:$E$9</definedName>
     <definedName name="typeofbuy">'Dmstc Stndrd Upld Tmplt'!$G$5</definedName>
     <definedName name="vendorstyledescription">'Dmstc Stndrd Upld Tmplt'!$C$5</definedName>
     <definedName name="vpn">'Dmstc Stndrd Upld Tmplt'!$B$5</definedName>
@@ -52,6 +55,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -338,8 +343,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="251">
   <si>
     <t>#</t>
   </si>
@@ -1144,12 +1171,15 @@
   <si>
     <t xml:space="preserve">Shape </t>
   </si>
+  <si>
+    <t>DD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1215,6 +1245,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
+      <name val="Roboto"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1451,7 +1488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1632,6 +1669,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2021,26 +2059,26 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="D85" sqref="D85"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="5.15625" style="26" customWidth="1"/>
-    <col min="2" max="2" width="27.15625" style="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="44.41796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="66.578125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="14.83984375" style="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.41796875" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.15625" style="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.41796875" style="28" customWidth="1"/>
-    <col min="10" max="10" width="15.41796875" style="26" customWidth="1"/>
-    <col min="11" max="11" width="14.83984375" style="26" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" style="26" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.5703125" style="26" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="28" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="26" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" style="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" ht="43.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2075,7 +2113,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" ht="28.9" hidden="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2110,7 +2148,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="11" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" s="11" customFormat="1" ht="28.9">
       <c r="A3" s="5">
         <v>5</v>
       </c>
@@ -2145,7 +2183,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="94.5" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" ht="94.5" hidden="1" customHeight="1">
       <c r="A4" s="5">
         <v>6</v>
       </c>
@@ -2180,7 +2218,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" hidden="1">
       <c r="A5" s="5">
         <v>7</v>
       </c>
@@ -2215,7 +2253,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" ht="28.9" hidden="1">
       <c r="A6" s="5">
         <v>10</v>
       </c>
@@ -2250,7 +2288,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" hidden="1">
       <c r="A7" s="5">
         <v>11</v>
       </c>
@@ -2285,7 +2323,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" ht="28.9" hidden="1">
       <c r="A8" s="5">
         <v>13</v>
       </c>
@@ -2320,7 +2358,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" hidden="1">
       <c r="A9" s="5">
         <v>15</v>
       </c>
@@ -2355,7 +2393,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11">
       <c r="A10" s="5">
         <v>16</v>
       </c>
@@ -2390,7 +2428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" hidden="1">
       <c r="A11" s="5">
         <v>17</v>
       </c>
@@ -2425,7 +2463,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" hidden="1">
       <c r="A12" s="5">
         <v>18</v>
       </c>
@@ -2460,7 +2498,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" hidden="1">
       <c r="A13" s="5">
         <v>19</v>
       </c>
@@ -2495,7 +2533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" hidden="1">
       <c r="A14" s="5">
         <v>20</v>
       </c>
@@ -2530,7 +2568,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" hidden="1">
       <c r="A15" s="5">
         <v>21</v>
       </c>
@@ -2565,7 +2603,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" hidden="1">
       <c r="A16" s="5">
         <v>22</v>
       </c>
@@ -2600,7 +2638,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" s="16" customFormat="1" hidden="1">
       <c r="A17" s="5">
         <v>23</v>
       </c>
@@ -2633,7 +2671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" hidden="1">
       <c r="A18" s="5">
         <v>24</v>
       </c>
@@ -2668,7 +2706,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" hidden="1">
       <c r="A19" s="5">
         <v>25</v>
       </c>
@@ -2703,7 +2741,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" hidden="1">
       <c r="A20" s="5">
         <v>26</v>
       </c>
@@ -2738,7 +2776,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" hidden="1">
       <c r="A21" s="5">
         <v>27</v>
       </c>
@@ -2773,7 +2811,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" hidden="1">
       <c r="A22" s="5">
         <v>28</v>
       </c>
@@ -2808,7 +2846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" hidden="1">
       <c r="A23" s="5">
         <v>29</v>
       </c>
@@ -2843,7 +2881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" hidden="1">
       <c r="A24" s="5">
         <v>30</v>
       </c>
@@ -2878,7 +2916,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" hidden="1">
       <c r="A25" s="5">
         <v>31</v>
       </c>
@@ -2913,7 +2951,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11">
       <c r="A26" s="5">
         <v>32</v>
       </c>
@@ -2948,7 +2986,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:11" hidden="1">
       <c r="A27" s="5">
         <v>33</v>
       </c>
@@ -2981,7 +3019,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:11" hidden="1">
       <c r="A28" s="5">
         <v>34</v>
       </c>
@@ -3016,7 +3054,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:11" ht="28.9" hidden="1">
       <c r="A29" s="5">
         <v>35</v>
       </c>
@@ -3051,7 +3089,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:11" hidden="1">
       <c r="A30" s="5">
         <v>36</v>
       </c>
@@ -3086,7 +3124,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11">
       <c r="A31" s="5">
         <v>37</v>
       </c>
@@ -3121,7 +3159,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:11" ht="28.9" hidden="1">
       <c r="A32" s="5">
         <v>38</v>
       </c>
@@ -3156,7 +3194,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:11" hidden="1">
       <c r="A33" s="5">
         <v>39</v>
       </c>
@@ -3191,7 +3229,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:11" hidden="1">
       <c r="A34" s="5">
         <v>40</v>
       </c>
@@ -3226,7 +3264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:11" hidden="1">
       <c r="A35" s="5">
         <v>41</v>
       </c>
@@ -3261,7 +3299,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:11" hidden="1">
       <c r="A36" s="5">
         <v>42</v>
       </c>
@@ -3296,7 +3334,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:11" hidden="1">
       <c r="A37" s="5">
         <v>43</v>
       </c>
@@ -3331,7 +3369,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:11" ht="28.9" hidden="1">
       <c r="A38" s="5">
         <v>45</v>
       </c>
@@ -3364,7 +3402,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:11" hidden="1">
       <c r="A39" s="5">
         <v>46</v>
       </c>
@@ -3399,7 +3437,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:11" ht="28.9" hidden="1">
       <c r="A40" s="5">
         <v>47</v>
       </c>
@@ -3434,7 +3472,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:11" ht="28.9" hidden="1">
       <c r="A41" s="5">
         <v>49</v>
       </c>
@@ -3469,7 +3507,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:11" hidden="1">
       <c r="A42" s="5">
         <v>50</v>
       </c>
@@ -3504,7 +3542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:11">
       <c r="A43" s="5">
         <v>51</v>
       </c>
@@ -3539,7 +3577,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:11" ht="43.15">
       <c r="A44" s="5">
         <v>52</v>
       </c>
@@ -3574,7 +3612,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:11" ht="43.15" hidden="1">
       <c r="A45" s="5">
         <v>55</v>
       </c>
@@ -3609,7 +3647,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:11" ht="28.9" hidden="1">
       <c r="A46" s="5">
         <v>57</v>
       </c>
@@ -3644,7 +3682,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:11" ht="28.9" hidden="1">
       <c r="A47" s="5">
         <v>58</v>
       </c>
@@ -3679,7 +3717,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:11" hidden="1">
       <c r="A48" s="5">
         <v>61</v>
       </c>
@@ -3714,7 +3752,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:11" ht="28.9" hidden="1">
       <c r="A49" s="5">
         <v>62</v>
       </c>
@@ -3747,7 +3785,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:11" ht="28.9" hidden="1">
       <c r="A50" s="5">
         <v>63</v>
       </c>
@@ -3782,7 +3820,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:11" ht="28.9" hidden="1">
       <c r="A51" s="5">
         <v>66</v>
       </c>
@@ -3817,7 +3855,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:11" hidden="1">
       <c r="A52" s="5">
         <v>76</v>
       </c>
@@ -3852,7 +3890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:11" hidden="1">
       <c r="A53" s="5">
         <v>77</v>
       </c>
@@ -3885,7 +3923,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:11" hidden="1">
       <c r="A54" s="5">
         <v>78</v>
       </c>
@@ -3918,7 +3956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:11" hidden="1">
       <c r="A55" s="5">
         <v>83</v>
       </c>
@@ -3953,7 +3991,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:11" hidden="1">
       <c r="A56" s="5">
         <v>84</v>
       </c>
@@ -3988,7 +4026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:11" ht="28.9" hidden="1">
       <c r="A57" s="5">
         <v>85</v>
       </c>
@@ -4023,7 +4061,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:11" hidden="1">
       <c r="A58" s="5">
         <v>90</v>
       </c>
@@ -4058,7 +4096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="16" customFormat="1" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:11" s="16" customFormat="1" hidden="1">
       <c r="A59" s="5">
         <v>92</v>
       </c>
@@ -4093,7 +4131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="60" hidden="1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:11" ht="60" hidden="1" customHeight="1">
       <c r="A60" s="5">
         <v>93</v>
       </c>
@@ -4128,7 +4166,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:11" hidden="1">
       <c r="A61" s="5">
         <v>98</v>
       </c>
@@ -4163,7 +4201,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:11" hidden="1">
       <c r="A62" s="5">
         <v>101</v>
       </c>
@@ -4198,7 +4236,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:11" hidden="1">
       <c r="A63" s="5">
         <v>102</v>
       </c>
@@ -4233,7 +4271,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="43.2" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:11" ht="43.15" hidden="1">
       <c r="A64" s="5">
         <v>103</v>
       </c>
@@ -4268,7 +4306,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:11" hidden="1">
       <c r="A65" s="5">
         <v>104</v>
       </c>
@@ -4303,7 +4341,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:11" hidden="1">
       <c r="A66" s="5">
         <v>105</v>
       </c>
@@ -4336,7 +4374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:11" hidden="1">
       <c r="A67" s="5">
         <v>106</v>
       </c>
@@ -4371,7 +4409,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:11" hidden="1">
       <c r="A68" s="5">
         <v>116</v>
       </c>
@@ -4406,7 +4444,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:11" hidden="1">
       <c r="A69" s="5">
         <v>117</v>
       </c>
@@ -4441,7 +4479,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:11" hidden="1">
       <c r="A70" s="5">
         <v>118</v>
       </c>
@@ -4476,7 +4514,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:11" hidden="1">
       <c r="A71" s="5">
         <v>119</v>
       </c>
@@ -4511,7 +4549,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:11" ht="28.9" hidden="1">
       <c r="A72" s="5">
         <v>120</v>
       </c>
@@ -4546,7 +4584,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:11" hidden="1">
       <c r="A73" s="5">
         <v>121</v>
       </c>
@@ -4581,7 +4619,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:11" hidden="1">
       <c r="A74" s="5">
         <v>122</v>
       </c>
@@ -4616,7 +4654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:11" hidden="1">
       <c r="A75" s="5">
         <v>123</v>
       </c>
@@ -4651,7 +4689,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:11" hidden="1">
       <c r="A76" s="5">
         <v>125</v>
       </c>
@@ -4686,7 +4724,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:11" hidden="1">
       <c r="A77" s="5">
         <v>126</v>
       </c>
@@ -4721,7 +4759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:11" hidden="1">
       <c r="A78" s="5">
         <v>129</v>
       </c>
@@ -4756,7 +4794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:11" hidden="1">
       <c r="A79" s="5">
         <v>130</v>
       </c>
@@ -4791,7 +4829,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:11" hidden="1">
       <c r="A80" s="5">
         <v>131</v>
       </c>
@@ -4826,7 +4864,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:11" ht="28.9">
       <c r="A81" s="5">
         <v>132</v>
       </c>
@@ -4861,7 +4899,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:11" hidden="1">
       <c r="A82" s="5">
         <v>133</v>
       </c>
@@ -4896,7 +4934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:11" hidden="1">
       <c r="A83" s="5">
         <v>138</v>
       </c>
@@ -4931,7 +4969,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:11" hidden="1">
       <c r="A84" s="5">
         <v>139</v>
       </c>
@@ -4966,7 +5004,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:11">
       <c r="A85" s="5">
         <v>141</v>
       </c>
@@ -5001,7 +5039,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:11" hidden="1">
       <c r="A86" s="5">
         <v>142</v>
       </c>
@@ -5036,7 +5074,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:11" hidden="1">
       <c r="A87" s="5">
         <v>147</v>
       </c>
@@ -5069,7 +5107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:11" hidden="1">
       <c r="A88" s="5">
         <v>148</v>
       </c>
@@ -5104,7 +5142,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:11" hidden="1">
       <c r="A89" s="5">
         <v>152</v>
       </c>
@@ -5137,7 +5175,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:11" hidden="1">
       <c r="A90" s="5">
         <v>153</v>
       </c>
@@ -5170,7 +5208,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:11" hidden="1">
       <c r="A91" s="5">
         <v>154</v>
       </c>
@@ -5203,7 +5241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:11" ht="28.9" hidden="1">
       <c r="A92" s="5">
         <v>155</v>
       </c>
@@ -5236,7 +5274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:11" s="24" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:11" s="24" customFormat="1" ht="28.9" hidden="1">
       <c r="A93" s="5">
         <v>158</v>
       </c>
@@ -5271,7 +5309,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:11" hidden="1">
       <c r="A94" s="5">
         <v>164</v>
       </c>
@@ -5304,7 +5342,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:11" hidden="1">
       <c r="A95" s="5">
         <v>165</v>
       </c>
@@ -5337,7 +5375,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:11" hidden="1">
       <c r="A96" s="5">
         <v>167</v>
       </c>
@@ -5372,7 +5410,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:11" hidden="1">
       <c r="A97" s="5">
         <v>168</v>
       </c>
@@ -5407,7 +5445,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:11" hidden="1">
       <c r="A98" s="5">
         <v>170</v>
       </c>
@@ -5442,7 +5480,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:11" hidden="1">
       <c r="A99" s="5">
         <v>173</v>
       </c>
@@ -5477,7 +5515,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:11" hidden="1">
       <c r="A100" s="5">
         <v>177</v>
       </c>
@@ -5512,7 +5550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:11" hidden="1">
       <c r="A101" s="5">
         <v>178</v>
       </c>
@@ -5600,76 +5638,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A17F3EB-F212-417F-BA00-A3FB97B2BF77}">
   <dimension ref="A1:CV5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="8.68359375"/>
-    <col min="2" max="2" width="9.41796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.41796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.41796875" style="37" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.41796875" style="38" customWidth="1"/>
-    <col min="8" max="8" width="9.41796875" style="40" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.578125" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.15625" style="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375"/>
+    <col min="2" max="2" width="9.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.42578125" style="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="38" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="40" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="39" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9" style="39" bestFit="1" customWidth="1"/>
-    <col min="13" max="18" width="8.41796875" style="39" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.41796875" style="39" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.15625" style="39" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="9.41796875" style="39" bestFit="1" customWidth="1"/>
-    <col min="24" max="30" width="8.41796875" style="39" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.15625" style="39" customWidth="1"/>
-    <col min="32" max="32" width="10.83984375" style="39" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.15625" style="39" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="12.68359375" style="39" customWidth="1"/>
+    <col min="13" max="18" width="8.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="21" max="23" width="9.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="24" max="30" width="8.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.140625" style="39" customWidth="1"/>
+    <col min="32" max="32" width="10.85546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" style="39" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="12.7109375" style="39" customWidth="1"/>
     <col min="35" max="35" width="11" style="38" customWidth="1"/>
-    <col min="36" max="36" width="8.68359375" style="38"/>
-    <col min="37" max="38" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="8.7109375" style="38"/>
+    <col min="37" max="38" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11" style="38" customWidth="1"/>
-    <col min="40" max="44" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.68359375" style="38"/>
-    <col min="46" max="46" width="8.578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="47" max="51" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.68359375" style="38"/>
-    <col min="53" max="55" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
+    <col min="40" max="44" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8.7109375" style="38"/>
+    <col min="46" max="46" width="8.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="47" max="51" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="8.7109375" style="38"/>
+    <col min="53" max="55" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="18" style="38" customWidth="1"/>
-    <col min="57" max="59" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="8.41796875" style="38" bestFit="1" customWidth="1"/>
-    <col min="61" max="63" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="13.578125" style="38" customWidth="1"/>
-    <col min="65" max="65" width="12.83984375" style="38" customWidth="1"/>
-    <col min="66" max="66" width="13.15625" style="38" customWidth="1"/>
-    <col min="67" max="67" width="11.83984375" style="38" customWidth="1"/>
-    <col min="68" max="68" width="15.83984375" style="38" customWidth="1"/>
-    <col min="69" max="69" width="13.15625" style="38" customWidth="1"/>
-    <col min="70" max="70" width="17.68359375" style="38" customWidth="1"/>
-    <col min="71" max="71" width="11.41796875" style="38" customWidth="1"/>
-    <col min="72" max="72" width="9.41796875" style="38" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="13.578125" style="38" customWidth="1"/>
-    <col min="75" max="75" width="8.578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="76" max="77" width="8.68359375" style="38"/>
-    <col min="78" max="80" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="8.41796875" style="38" bestFit="1" customWidth="1"/>
-    <col min="82" max="83" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="13.15625" style="38" customWidth="1"/>
-    <col min="85" max="86" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="8.41796875" style="38" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="10.578125" style="38" customWidth="1"/>
-    <col min="89" max="89" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="8.41796875" style="38" bestFit="1" customWidth="1"/>
-    <col min="91" max="91" width="10.15625" style="38" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="93" max="94" width="9.41796875" style="38" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="11.41796875" style="38" customWidth="1"/>
-    <col min="96" max="99" width="8.26171875" style="38" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="10.15625" style="38" bestFit="1" customWidth="1"/>
+    <col min="57" max="59" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="8.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="61" max="63" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.5703125" style="38" customWidth="1"/>
+    <col min="65" max="65" width="12.85546875" style="38" customWidth="1"/>
+    <col min="66" max="66" width="13.140625" style="38" customWidth="1"/>
+    <col min="67" max="67" width="11.85546875" style="38" customWidth="1"/>
+    <col min="68" max="68" width="15.85546875" style="38" customWidth="1"/>
+    <col min="69" max="69" width="13.140625" style="38" customWidth="1"/>
+    <col min="70" max="70" width="17.7109375" style="38" customWidth="1"/>
+    <col min="71" max="71" width="11.42578125" style="38" customWidth="1"/>
+    <col min="72" max="72" width="9.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="13.5703125" style="38" customWidth="1"/>
+    <col min="75" max="75" width="8.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="76" max="77" width="8.7109375" style="38"/>
+    <col min="78" max="80" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="8.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="82" max="83" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13.140625" style="38" customWidth="1"/>
+    <col min="85" max="86" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="8.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="10.5703125" style="38" customWidth="1"/>
+    <col min="89" max="89" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="8.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="10.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="93" max="94" width="9.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="11.42578125" style="38" customWidth="1"/>
+    <col min="96" max="99" width="8.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="10.140625" style="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:100" ht="43.15">
       <c r="A1" s="30" t="s">
         <v>5</v>
       </c>
@@ -5971,7 +6009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:100" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:100" ht="14.65" thickBot="1">
       <c r="A2" s="31" t="s">
         <v>1</v>
       </c>
@@ -6273,7 +6311,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:100">
       <c r="A3" s="31"/>
       <c r="B3" s="52" t="s">
         <v>17</v>
@@ -6573,7 +6611,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:100" s="29" customFormat="1" ht="57.9" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:100" s="29" customFormat="1" ht="57.95" thickBot="1">
       <c r="A4" s="31" t="s">
         <v>248</v>
       </c>
@@ -6601,8 +6639,9 @@
       <c r="I4" s="64" t="s">
         <v>194</v>
       </c>
-      <c r="J4" s="64" t="s">
-        <v>147</v>
+      <c r="J4" s="64">
+        <f>J12</f>
+        <v>0</v>
       </c>
       <c r="K4" s="64" t="s">
         <v>149</v>
@@ -6875,7 +6914,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:100" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:100" hidden="1">
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
       <c r="D5" s="47"/>
@@ -6988,6 +7027,75 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{028A8C3F-5960-4A04-A75A-F910C64FDA5F}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75">
+      <c r="F1" s="70" t="e" cm="1">
+        <f t="array" aca="1" ref="F1" ca="1">SheetName</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="str">
+        <f>'Dmstc Stndrd Upld Tmplt'!V4</f>
+        <v xml:space="preserve">Budget Month </v>
+      </c>
+      <c r="B2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6995,6 +7103,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007AA5452FB13DA84FABB9428584074F11" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7ef02b788f49ae2a7b323e42f377b017">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cc44513a-9740-48a8-b9a6-11a9236a0f51" xmlns:ns3="ab086da4-aeaa-470f-88f5-e96437a646bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e7382a5f6038dbc6f6e7efbc7d46eb3" ns2:_="" ns3:_="">
     <xsd:import namespace="cc44513a-9740-48a8-b9a6-11a9236a0f51"/>
@@ -7179,55 +7296,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7799FA91-D05F-41CA-9D85-32D7401AB4F3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="ab086da4-aeaa-470f-88f5-e96437a646bb"/>
-    <ds:schemaRef ds:uri="cc44513a-9740-48a8-b9a6-11a9236a0f51"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7799FA91-D05F-41CA-9D85-32D7401AB4F3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41DAFC0D-C589-4871-8EC2-037587728CED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cc44513a-9740-48a8-b9a6-11a9236a0f51"/>
-    <ds:schemaRef ds:uri="ab086da4-aeaa-470f-88f5-e96437a646bb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9149A93E-C697-4066-B609-D79D6821B8AF}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9149A93E-C697-4066-B609-D79D6821B8AF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41DAFC0D-C589-4871-8EC2-037587728CED}"/>
 </file>
</xml_diff>